<commit_message>
23 Nov 2022 commit only
</commit_message>
<xml_diff>
--- a/data-structure-algorithm/src/test/resources/INTERVIEW_FINAL450.xlsx
+++ b/data-structure-algorithm/src/test/resources/INTERVIEW_FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sutha\IdeaProjects\datastructure\data-structure-algorithm\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B37885D-8BE0-45BD-8287-C51FF18E27BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1495,12 +1495,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1516,7 +1522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1540,6 +1546,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1858,17 +1871,17 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,24 +1941,24 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>